<commit_message>
add : import to all menu (t1)
</commit_message>
<xml_diff>
--- a/public/template_barang.xlsx
+++ b/public/template_barang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Any Maya\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B12BB5E-1388-4D3A-8816-A0DE3E868C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3106BB7-A806-4CB0-9429-3A213B7D1FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{54A10731-DEAF-46BA-B8E7-6068D0A99889}"/>
   </bookViews>
@@ -433,7 +433,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>